<commit_message>
update import add more contract details.
</commit_message>
<xml_diff>
--- a/src/main/webapp/MemberImportTemplate.xlsx
+++ b/src/main/webapp/MemberImportTemplate.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26101"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -17,6 +17,9 @@
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -25,47 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="72">
-  <si>
-    <t>注意：红色列为必填项，登录用户名不能重复</t>
-    <rPh sb="0" eb="1">
-      <t>iyuj</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>xaq</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>gq</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>o</t>
-    </rPh>
-    <rPh sb="7" eb="8">
-      <t>ntff</t>
-    </rPh>
-    <rPh sb="9" eb="10">
-      <t>adm</t>
-    </rPh>
-    <rPh sb="11" eb="12">
-      <t>wgv</t>
-    </rPh>
-    <rPh sb="13" eb="14">
-      <t>etyn</t>
-    </rPh>
-    <rPh sb="15" eb="16">
-      <t>qk</t>
-    </rPh>
-    <rPh sb="16" eb="17">
-      <t>i</t>
-    </rPh>
-    <rPh sb="17" eb="18">
-      <t>ce</t>
-    </rPh>
-    <rPh sb="18" eb="19">
-      <t>tgtj</t>
-    </rPh>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
   <si>
     <t>合同日期</t>
     <rPh sb="0" eb="1">
@@ -572,33 +535,12 @@
     <t>法人</t>
   </si>
   <si>
-    <t>法人身份证号</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>联系人</t>
   </si>
   <si>
     <t>联系电话</t>
   </si>
   <si>
-    <t>第二联系人</t>
-  </si>
-  <si>
-    <t>第二联系电话</t>
-  </si>
-  <si>
-    <t>联系邮箱</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>传真</t>
-  </si>
-  <si>
-    <t>纳税人识别号</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>开户银行</t>
   </si>
   <si>
@@ -609,15 +551,6 @@
   </si>
   <si>
     <t>统一代码</t>
-  </si>
-  <si>
-    <t>是否新版营业执照</t>
-  </si>
-  <si>
-    <t>附件1（营业执照）</t>
-  </si>
-  <si>
-    <t>附件2（企业授权书）</t>
   </si>
   <si>
     <t>品牌</t>
@@ -640,17 +573,6 @@
     <t>001</t>
   </si>
   <si>
-    <t>福州泛泰锡</t>
-  </si>
-  <si>
-    <t>fzftxgs</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>15000033449</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>福州泛泰锡贸易有限公司</t>
   </si>
   <si>
@@ -660,9 +582,6 @@
     <t>0591-87559227</t>
   </si>
   <si>
-    <t>91350103066559931C</t>
-  </si>
-  <si>
     <t>中国建设银行福州市城南支行营业厅</t>
   </si>
   <si>
@@ -675,22 +594,12 @@
     <t>002</t>
   </si>
   <si>
-    <t>福州鑫和园</t>
-  </si>
-  <si>
-    <t>fzxhygs</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>福州鑫和园商贸有限公司</t>
   </si>
   <si>
     <t xml:space="preserve">张蒙君 </t>
   </si>
   <si>
-    <t>91350102579275045G</t>
-  </si>
-  <si>
     <t>中国银行五一广场支行</t>
   </si>
   <si>
@@ -698,14 +607,6 @@
   </si>
   <si>
     <t>福州市鼓楼区杨桥路99号三友大厦10层南单元</t>
-  </si>
-  <si>
-    <t>福州泛泰锡贸易有限公司</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>福州鑫和园商贸有限公司</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>常州化工常润</t>
@@ -744,28 +645,56 @@
     <t>qr.png</t>
   </si>
   <si>
+    <t>2017/11/02</t>
+  </si>
+  <si>
+    <t>注意：红色列为必填项，登录用户名不能重复</t>
+  </si>
+  <si>
+    <t>申请日期</t>
+  </si>
+  <si>
+    <t>法人身份证号</t>
+  </si>
+  <si>
     <t>2017/11/01</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>2017/11/02</t>
-  </si>
-  <si>
-    <t>申请日期</t>
-    <rPh sb="0" eb="1">
-      <t>jhy</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>jja</t>
-    </rPh>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>福州泛泰锡2</t>
+  </si>
+  <si>
+    <t>fzftxgs2</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>福州泛泰锡贸易有限公司2</t>
+  </si>
+  <si>
+    <t>91350103066559932C</t>
+  </si>
+  <si>
+    <t>福州鑫和园2</t>
+  </si>
+  <si>
+    <t>fzxhygs2</t>
+  </si>
+  <si>
+    <t>福州鑫和园商贸有限公司2</t>
+  </si>
+  <si>
+    <t>91350102579275046G</t>
+  </si>
+  <si>
+    <t>83229502</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -790,15 +719,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Abadi MT Condensed Extra Bold"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Abadi MT Condensed Extra Bold"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -821,7 +760,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -835,7 +774,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -845,6 +784,16 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1126,7 +1075,7 @@
   <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -1140,218 +1089,191 @@
     <col min="8" max="8" width="23.6640625" style="3" customWidth="1"/>
     <col min="9" max="9" width="18.5" style="3" customWidth="1"/>
     <col min="10" max="19" width="10.83203125" style="3"/>
-    <col min="20" max="20" width="10.83203125" style="2"/>
+    <col min="20" max="20" width="9.5" style="2" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="17.5" style="3" bestFit="1" customWidth="1"/>
     <col min="22" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A1" s="12"/>
+      <c r="B1" s="12"/>
       <c r="C1" s="9" t="s">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
+      <c r="H1" s="2"/>
       <c r="I1" s="9"/>
       <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
     </row>
     <row r="2" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="J2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="K2" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="L2" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="M2" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="N2" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="O2" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="U2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="V2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="W2" s="4" t="s">
-        <v>38</v>
-      </c>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
     </row>
     <row r="3" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" s="4">
-        <v>123456</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="S3" s="4" t="s">
-        <v>51</v>
-      </c>
+      <c r="A3" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
       <c r="T3" s="4"/>
-      <c r="U3" s="4" t="s">
-        <v>48</v>
-      </c>
+      <c r="U3" s="4"/>
       <c r="V3" s="4"/>
       <c r="W3" s="4"/>
       <c r="X3" s="4"/>
     </row>
     <row r="4" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E4" s="4">
-        <v>123456</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G4" s="4" t="s">
+      <c r="A4" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K4" s="4">
-        <v>83229502</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="M4" s="4">
-        <v>83229502</v>
-      </c>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="R4" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="S4" s="4" t="s">
-        <v>60</v>
-      </c>
+      <c r="H4" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="N4" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="O4" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
       <c r="T4" s="4"/>
-      <c r="U4" s="4" t="s">
-        <v>57</v>
-      </c>
+      <c r="U4" s="4"/>
       <c r="V4" s="4"/>
       <c r="W4" s="4"/>
       <c r="X4" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C1:J1"/>
-  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1377,7 +1299,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="103" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -1398,55 +1320,55 @@
     </row>
     <row r="2" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2" t="s">
-        <v>40</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" t="s">
         <v>14</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.15">
@@ -1457,28 +1379,28 @@
         <v>42998</v>
       </c>
       <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" t="s">
         <v>45</v>
       </c>
-      <c r="D3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F3" t="s">
-        <v>64</v>
-      </c>
       <c r="G3" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="H3" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="I3" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="J3" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="K3">
         <v>250</v>
@@ -1499,7 +1421,7 @@
         <v>42998</v>
       </c>
       <c r="Q3" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>